<commit_message>
Changed scheduling so that the labs are scheduled first as labs are more valuable than classes
</commit_message>
<xml_diff>
--- a/example_students.xlsx
+++ b/example_students.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B9DD88-AF0C-47A0-A401-18B1D63C9BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DB7C1E-5F92-4DD8-BCBF-23D44707D398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="2700" windowWidth="21600" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated excel files to have real student names to be displayed on the cohorts screen
</commit_message>
<xml_diff>
--- a/example_students.xlsx
+++ b/example_students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED77FFE-0546-440F-A65B-5A409C6D43A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C0BE4D-DADA-4896-AD50-299AE4C88670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="3615" windowWidth="21600" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="4395" windowWidth="21600" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Program</t>
-  </si>
-  <si>
-    <t>Fname Lname</t>
   </si>
   <si>
     <t>PCOM</t>
@@ -72,6 +69,81 @@
   </si>
   <si>
     <t>GL</t>
+  </si>
+  <si>
+    <t>Matt Smith</t>
+  </si>
+  <si>
+    <t>George Johnson</t>
+  </si>
+  <si>
+    <t>Matt Cramer</t>
+  </si>
+  <si>
+    <t>George Smith</t>
+  </si>
+  <si>
+    <t>Sam Smith</t>
+  </si>
+  <si>
+    <t>Ann Mikar</t>
+  </si>
+  <si>
+    <t>Sam Mikar</t>
+  </si>
+  <si>
+    <t>Sam Johnson</t>
+  </si>
+  <si>
+    <t>Ann Smith</t>
+  </si>
+  <si>
+    <t>Ann Stevenson</t>
+  </si>
+  <si>
+    <t>Jennifer Cramer</t>
+  </si>
+  <si>
+    <t>Sam Stevenson</t>
+  </si>
+  <si>
+    <t>Jennifer Johnson</t>
+  </si>
+  <si>
+    <t>Jennifer Stevenson</t>
+  </si>
+  <si>
+    <t>George Mikar</t>
+  </si>
+  <si>
+    <t>Matt Mikar</t>
+  </si>
+  <si>
+    <t>Sam Cramer</t>
+  </si>
+  <si>
+    <t>Matt Johnson</t>
+  </si>
+  <si>
+    <t>Jennifer Smith</t>
+  </si>
+  <si>
+    <t>Ann Cramer</t>
+  </si>
+  <si>
+    <t>Matt Stevenson</t>
+  </si>
+  <si>
+    <t>Jennifer Mikar</t>
+  </si>
+  <si>
+    <t>George Stevenson</t>
+  </si>
+  <si>
+    <t>George Cramer</t>
+  </si>
+  <si>
+    <t>Ann Johnson</t>
   </si>
 </sst>
 </file>
@@ -425,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,16 +528,16 @@
         <v>3104535</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -473,16 +545,16 @@
         <v>3104536</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,16 +562,16 @@
         <v>3104537</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -507,16 +579,16 @@
         <v>3104538</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -524,16 +596,16 @@
         <v>3104539</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,16 +613,16 @@
         <v>3104540</v>
       </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,16 +630,16 @@
         <v>3104541</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,16 +647,16 @@
         <v>3104542</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,16 +664,16 @@
         <v>3104543</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -609,16 +681,16 @@
         <v>3104544</v>
       </c>
       <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,16 +698,16 @@
         <v>3104545</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,16 +715,16 @@
         <v>3104546</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,16 +732,16 @@
         <v>3104547</v>
       </c>
       <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,16 +749,16 @@
         <v>3104548</v>
       </c>
       <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,16 +766,16 @@
         <v>3104549</v>
       </c>
       <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,16 +783,16 @@
         <v>3104550</v>
       </c>
       <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,16 +800,16 @@
         <v>3104551</v>
       </c>
       <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,16 +817,16 @@
         <v>3104552</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,16 +834,16 @@
         <v>3104553</v>
       </c>
       <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,16 +851,16 @@
         <v>3104554</v>
       </c>
       <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,16 +868,16 @@
         <v>3104555</v>
       </c>
       <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,16 +885,16 @@
         <v>3104556</v>
       </c>
       <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
         <v>5</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,16 +902,16 @@
         <v>3104557</v>
       </c>
       <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -847,16 +919,16 @@
         <v>3104558</v>
       </c>
       <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -864,16 +936,16 @@
         <v>3104559</v>
       </c>
       <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>5</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -881,16 +953,16 @@
         <v>3104560</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
         <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,16 +970,16 @@
         <v>3104561</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>9</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,16 +987,16 @@
         <v>3104562</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
         <v>9</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,16 +1004,16 @@
         <v>3104563</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,16 +1021,16 @@
         <v>3104564</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
         <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -966,16 +1038,16 @@
         <v>3104565</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
         <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -983,16 +1055,16 @@
         <v>3104566</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>9</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,16 +1072,16 @@
         <v>3104567</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
         <v>9</v>
-      </c>
-      <c r="E34" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1017,16 +1089,16 @@
         <v>3104568</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
         <v>9</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,16 +1106,16 @@
         <v>3104569</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
         <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1051,16 +1123,16 @@
         <v>3104570</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
         <v>9</v>
-      </c>
-      <c r="E37" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,16 +1140,16 @@
         <v>3104571</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
         <v>9</v>
-      </c>
-      <c r="E38" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,16 +1157,16 @@
         <v>3104572</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,16 +1174,16 @@
         <v>3104573</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,16 +1191,16 @@
         <v>3104574</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,16 +1208,16 @@
         <v>3104575</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1153,16 +1225,16 @@
         <v>3104576</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1170,16 +1242,16 @@
         <v>3104577</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1187,16 +1259,16 @@
         <v>3104578</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1204,16 +1276,16 @@
         <v>3104579</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,16 +1293,16 @@
         <v>3104580</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,16 +1310,16 @@
         <v>3104581</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,16 +1327,16 @@
         <v>3104582</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,16 +1344,16 @@
         <v>3104583</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1289,16 +1361,16 @@
         <v>3104584</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,16 +1378,16 @@
         <v>3104585</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,16 +1395,16 @@
         <v>3104586</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,16 +1412,16 @@
         <v>3104587</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,16 +1429,16 @@
         <v>3104588</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,16 +1446,16 @@
         <v>3104589</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1391,16 +1463,16 @@
         <v>3104590</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,16 +1480,16 @@
         <v>3104591</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,16 +1497,16 @@
         <v>3104592</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,16 +1514,16 @@
         <v>3104593</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,16 +1531,16 @@
         <v>3104594</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,16 +1548,16 @@
         <v>3104595</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1493,16 +1565,16 @@
         <v>3104596</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,16 +1582,16 @@
         <v>3104597</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,16 +1599,16 @@
         <v>3104598</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1544,16 +1616,16 @@
         <v>3104599</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1561,16 +1633,16 @@
         <v>3104600</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,16 +1650,16 @@
         <v>3104601</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1595,16 +1667,16 @@
         <v>3104602</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1612,16 +1684,16 @@
         <v>3104603</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1629,16 +1701,16 @@
         <v>3104604</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,16 +1718,16 @@
         <v>3104605</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1663,16 +1735,16 @@
         <v>3104606</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1680,16 +1752,16 @@
         <v>3104607</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1697,16 +1769,16 @@
         <v>3104608</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,16 +1786,16 @@
         <v>3104609</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,16 +1803,16 @@
         <v>3104610</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,16 +1820,16 @@
         <v>3104611</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,16 +1837,16 @@
         <v>3104612</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,16 +1854,16 @@
         <v>3104613</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1799,16 +1871,16 @@
         <v>3104614</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1816,16 +1888,16 @@
         <v>3104615</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1833,16 +1905,16 @@
         <v>3104616</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1850,16 +1922,16 @@
         <v>3104617</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1867,16 +1939,16 @@
         <v>3104618</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1884,16 +1956,16 @@
         <v>3104619</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1901,16 +1973,16 @@
         <v>3104620</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1918,16 +1990,16 @@
         <v>3104621</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -1935,16 +2007,16 @@
         <v>3104622</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1952,16 +2024,16 @@
         <v>3104623</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1969,16 +2041,16 @@
         <v>3104624</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -1986,16 +2058,16 @@
         <v>3104625</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2003,16 +2075,16 @@
         <v>3104626</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2020,16 +2092,16 @@
         <v>3104627</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E94" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2037,16 +2109,16 @@
         <v>3104628</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E95" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2054,16 +2126,16 @@
         <v>3104629</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2071,16 +2143,16 @@
         <v>3104630</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E97" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2088,16 +2160,16 @@
         <v>3104631</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2105,1410 +2177,1410 @@
         <v>3104632</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E99" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>3104572</v>
+        <v>3104633</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>3104573</v>
+        <v>3104634</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>3104574</v>
+        <v>3104635</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>3104575</v>
+        <v>3104636</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>3104576</v>
+        <v>3104637</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C104">
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>3104577</v>
+        <v>3104638</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>3104578</v>
+        <v>3104639</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>3104579</v>
+        <v>3104640</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C107">
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>3104580</v>
+        <v>3104641</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C108">
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>3104581</v>
+        <v>3104642</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>3104582</v>
+        <v>3104643</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C110">
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>3104583</v>
+        <v>3104644</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>3104584</v>
+        <v>3104645</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C112">
         <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>3104585</v>
+        <v>3104646</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>3104586</v>
+        <v>3104647</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C114">
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>3104587</v>
+        <v>3104648</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C115">
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>3104588</v>
+        <v>3104649</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>3104589</v>
+        <v>3104650</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E117" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>3104590</v>
+        <v>3104651</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>3104591</v>
+        <v>3104652</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E119" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>3104592</v>
+        <v>3104653</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>3104593</v>
+        <v>3104654</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E121" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>3104594</v>
+        <v>3104655</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C122">
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>3104595</v>
+        <v>3104656</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>3104596</v>
+        <v>3104657</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C124">
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E124" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>3104597</v>
+        <v>3104658</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C125">
         <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E125" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>3104598</v>
+        <v>3104659</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C126">
         <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>3104599</v>
+        <v>3104660</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C127">
         <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>3104600</v>
+        <v>3104661</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C128">
         <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>3104601</v>
+        <v>3104662</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C129">
         <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E129" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>3104602</v>
+        <v>3104663</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C130">
         <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E130" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>3104603</v>
+        <v>3104664</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C131">
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E131" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>3104604</v>
+        <v>3104665</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C132">
         <v>2</v>
       </c>
       <c r="D132" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E132" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>3104605</v>
+        <v>3104666</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C133">
         <v>2</v>
       </c>
       <c r="D133" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>3104606</v>
+        <v>3104667</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C134">
         <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E134" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>3104607</v>
+        <v>3104668</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C135">
         <v>2</v>
       </c>
       <c r="D135" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>3104608</v>
+        <v>3104669</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C136">
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E136" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>3104609</v>
+        <v>3104670</v>
       </c>
       <c r="B137" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C137">
         <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>3104610</v>
+        <v>3104671</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C138">
         <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E138" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>3104611</v>
+        <v>3104672</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C139">
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E139" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>3104612</v>
+        <v>3104673</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C140">
         <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E140" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>3104613</v>
+        <v>3104674</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C141">
         <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E141" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>3104614</v>
+        <v>3104675</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C142">
         <v>2</v>
       </c>
       <c r="D142" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>3104615</v>
+        <v>3104676</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C143">
         <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E143" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>3104616</v>
+        <v>3104677</v>
       </c>
       <c r="B144" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C144">
         <v>2</v>
       </c>
       <c r="D144" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E144" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>3104617</v>
+        <v>3104678</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C145">
         <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E145" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>3104618</v>
+        <v>3104679</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C146">
         <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E146" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>3104619</v>
+        <v>3104680</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C147">
         <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E147" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>3104620</v>
+        <v>3104681</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C148">
         <v>2</v>
       </c>
       <c r="D148" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E148" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>3104621</v>
+        <v>3104682</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C149">
         <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E149" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>3104622</v>
+        <v>3104683</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C150">
         <v>2</v>
       </c>
       <c r="D150" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E150" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>3104623</v>
+        <v>3104684</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C151">
         <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E151" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>3104624</v>
+        <v>3104685</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C152">
         <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E152" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>3104625</v>
+        <v>3104686</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C153">
         <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E153" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>3104626</v>
+        <v>3104687</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C154">
         <v>2</v>
       </c>
       <c r="D154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E154" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>3104627</v>
+        <v>3104688</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C155">
         <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E155" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>3104628</v>
+        <v>3104689</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C156">
         <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E156" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>3104629</v>
+        <v>3104690</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C157">
         <v>2</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E157" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>3104630</v>
+        <v>3104691</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C158">
         <v>2</v>
       </c>
       <c r="D158" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E158" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>3104631</v>
+        <v>3104692</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C159">
         <v>2</v>
       </c>
       <c r="D159" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E159" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>3104632</v>
+        <v>3104693</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C160">
         <v>2</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E160" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>3104633</v>
+        <v>3104694</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C161">
         <v>2</v>
       </c>
       <c r="D161" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E161" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>3104634</v>
+        <v>3104695</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C162">
         <v>2</v>
       </c>
       <c r="D162" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E162" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>3104635</v>
+        <v>3104696</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C163">
         <v>2</v>
       </c>
       <c r="D163" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E163" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>3104636</v>
+        <v>3104697</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C164">
         <v>2</v>
       </c>
       <c r="D164" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E164" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>3104637</v>
+        <v>3104698</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C165">
         <v>2</v>
       </c>
       <c r="D165" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E165" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>3104638</v>
+        <v>3104699</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C166">
         <v>2</v>
       </c>
       <c r="D166" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E166" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>3104639</v>
+        <v>3104700</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C167">
         <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E167" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>3104640</v>
+        <v>3104701</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C168">
         <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E168" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>3104641</v>
+        <v>3104702</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C169">
         <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E169" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>3104642</v>
+        <v>3104703</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C170">
         <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E170" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>3104643</v>
+        <v>3104704</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C171">
         <v>2</v>
       </c>
       <c r="D171" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E171" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>3104644</v>
+        <v>3104705</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C172">
         <v>2</v>
       </c>
       <c r="D172" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E172" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>3104645</v>
+        <v>3104706</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C173">
         <v>2</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E173" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>3104646</v>
+        <v>3104707</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C174">
         <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E174" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>3104647</v>
+        <v>3104708</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C175">
         <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E175" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>3104648</v>
+        <v>3104709</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C176">
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E176" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>3104649</v>
+        <v>3104710</v>
       </c>
       <c r="B177" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C177">
         <v>2</v>
       </c>
       <c r="D177" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E177" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>3104650</v>
+        <v>3104711</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C178">
         <v>2</v>
       </c>
       <c r="D178" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E178" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>3104651</v>
+        <v>3104712</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C179">
         <v>2</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E179" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>3104652</v>
+        <v>3104713</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C180">
         <v>2</v>
       </c>
       <c r="D180" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E180" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>3104653</v>
+        <v>3104714</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C181">
         <v>2</v>
       </c>
       <c r="D181" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E181" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>